<commit_message>
lunes 8 cambios anteriores
</commit_message>
<xml_diff>
--- a/cuadros/7.discriminacion.xlsx
+++ b/cuadros/7.discriminacion.xlsx
@@ -8,12 +8,17 @@
   <sheets>
     <sheet name="q62_descendencia" r:id="rId3" sheetId="1"/>
     <sheet name="q63_genero" r:id="rId4" sheetId="2"/>
+    <sheet name="q64_edad_abs" r:id="rId5" sheetId="3"/>
+    <sheet name="q64_edad_freq" r:id="rId6" sheetId="4"/>
+    <sheet name="grafico_7.10" r:id="rId7" sheetId="5"/>
+    <sheet name="enam2020_genero" r:id="rId8" sheetId="6"/>
+    <sheet name="niveled" r:id="rId9" sheetId="7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>q62_new</t>
   </si>
@@ -79,6 +84,69 @@
   </si>
   <si>
     <t>Varón</t>
+  </si>
+  <si>
+    <t>q64_violencia_fuerza_seguridad</t>
+  </si>
+  <si>
+    <t>18-34</t>
+  </si>
+  <si>
+    <t>35-54</t>
+  </si>
+  <si>
+    <t>55+</t>
+  </si>
+  <si>
+    <t>Prefiero no responder</t>
+  </si>
+  <si>
+    <t>Sí, alguna vez</t>
+  </si>
+  <si>
+    <t>Sí, frecuentemente</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>q64_violencia_fuerza_seguridad/edad_2020</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>q56_violencia_genero</t>
+  </si>
+  <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>No quiero responder</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Tal vez</t>
+  </si>
+  <si>
+    <t>Hasta secundario incompleto</t>
+  </si>
+  <si>
+    <t>Secundario completo</t>
+  </si>
+  <si>
+    <t>Superior completo y más</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -357,4 +425,505 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1072.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1454.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1228.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="n">
+        <v>247.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>268.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>125.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>34.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>100.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3753.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>852.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>304.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2527.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="n">
+        <v>139.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>77.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="n">
+        <v>640.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>187.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>366.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>25.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="n">
+        <v>962.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>810.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>43.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>277.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" t="n">
+        <v>82.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="n">
+        <v>380.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>427.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1208.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>551.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>543.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="n">
+        <v>897.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>657.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>580.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>